<commit_message>
[MS-ONESTORE] Add capture codes in S02 and update RS
</commit_message>
<xml_diff>
--- a/FileSyncandWOPI/Docs/MS-ONESTORE/MS-ONESTORE_RequirementSpecification.xlsx
+++ b/FileSyncandWOPI/Docs/MS-ONESTORE/MS-ONESTORE_RequirementSpecification.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21DF3B59-E4F9-4D68-A5AD-0A0BEE43A05C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4E3A696-0BD7-4429-A44E-9C1E0416BECD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="14670" windowHeight="8325" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="14670" windowHeight="8325" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="2" r:id="rId1"/>
@@ -6491,12 +6491,6 @@
     <t>[In GlobalIdTableEntry2FNDX] [iIndexMapTo] MUST be unique relative to the other indices in this global identification table specified by FileNode structures with the value of the FileNode.FileNodeID field equal to 0x024 (GlobalIdTableEntryFNDX structure), 0x25 (GlobalIdTableEntry2FNDX structure), and 0x26 (GlobalIdTableEntry3FNDX structure).</t>
   </si>
   <si>
-    <t>[In GlobalIdTableEntry2FNDX] The iIndexMapTo is defferent in two global identification table specified by FileNode structures with the value of the FileNode.FileNodeID field equal to 0x024 (GlobalIdTableEntryFNDX structure), 0x25 (GlobalIdTableEntry2FNDX structure), and 0x26 (GlobalIdTableEntry3FNDX structure).</t>
-  </si>
-  <si>
-    <t>[In GlobalIdTableEntryFNDX]  The indexes in two global identification table specified by FileNode structures with the values of the FileNode.FileNodeID fields equal to 0x024 (GlobalIdTableEntryFNDX structure), 0x25 (GlobalIdTableEntry2FNDX structure), and 0x26 (GlobalIdTableEntry3FNDX structure) are different.</t>
-  </si>
-  <si>
     <t>MS-ONESTORE_R55901</t>
   </si>
   <si>
@@ -6513,9 +6507,6 @@
   </si>
   <si>
     <t>Partial derived by requirement: MS-ONESTORE_R57001</t>
-  </si>
-  <si>
-    <t>[In GlobalIdTableEntry3FNDX] The indices from the value of iIndexCopyToStart to the value of (iIndexCopyToStart + cEntriesToCopy – 1) are different in two global identification table specified by FileNode structures with the values of the FileNode.FileNodeID field equal to 0x024 (GlobalIdTableEntryFNDX structure), 0x025 (GlobalIdTableEntry2FNDX structure), and 0x026 (GlobalIdTableEntry3FNDX structure).</t>
   </si>
   <si>
     <t>[In RevisionRoleDeclarationFND] [rid] MUST match the value of the RevisionManifestStart4FND.rid field,  RevisionManifestStart6FND.rid field or RevisionManifestStart7FND.base.rid field of one of preceding revision manifests (section 2.1.9) in the current revision manifest list (section 2.1.10).</t>
@@ -6765,6 +6756,16 @@
   <si>
     <t>[In RevisionManifestStart6FND] [ridDependent] Otherwise[If the value is not "{{00000000-0000-0000-0000-000000000000}, 0}"], this value MUST be equal to [the RevisionManifestStart6FND.rid field or] the RevisionManifestStart7FND.base.rid field of a previous revision manifest within this revision manifest list.</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In GlobalIdTableEntryFNDX]  The indexes in global identification table specified by FileNode structures with the values of the FileNode.FileNodeID fields equal to 0x024 (GlobalIdTableEntryFNDX structure) is different.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In GlobalIdTableEntry2FNDX] The iIndexMapTo is different in global identification table specified by FileNode structures with the value of the FileNode.FileNodeID field equal to 0x25 (GlobalIdTableEntry2FNDX structure).</t>
+  </si>
+  <si>
+    <t>[In GlobalIdTableEntry3FNDX] The indices from the value of iIndexCopyToStart to the value of (iIndexCopyToStart + cEntriesToCopy – 1) is different in global identification table specified by FileNode structures with the values of the FileNode.FileNodeID field equal to 0x026 (GlobalIdTableEntry3FNDX structure).</t>
   </si>
 </sst>
 </file>
@@ -6834,7 +6835,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -6862,12 +6863,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6985,7 +6980,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -7063,24 +7058,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -7104,6 +7081,21 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -9633,7 +9625,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>2123</v>
+        <v>2120</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -9658,31 +9650,31 @@
       <c r="J3" s="4"/>
     </row>
     <row r="4" spans="1:15" ht="21" x14ac:dyDescent="0.25">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
+      <c r="B4" s="41"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
       <c r="J4" s="4"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="38"/>
-      <c r="I5" s="38"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="45"/>
       <c r="J5" s="4"/>
       <c r="O5" s="32"/>
     </row>
@@ -9690,96 +9682,96 @@
       <c r="A6" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="43" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="36"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
-      <c r="G6" s="36"/>
-      <c r="H6" s="36"/>
-      <c r="I6" s="36"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43"/>
       <c r="J6" s="4"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="35"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
-      <c r="H7" s="35"/>
-      <c r="I7" s="35"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="42"/>
+      <c r="I7" s="42"/>
       <c r="J7" s="4"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="35" t="s">
+      <c r="B8" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="35"/>
-      <c r="I8" s="35"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="42"/>
       <c r="J8" s="4"/>
     </row>
     <row r="9" spans="1:15" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="43" t="s">
+      <c r="B9" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="44"/>
-      <c r="D9" s="44"/>
-      <c r="E9" s="44"/>
-      <c r="F9" s="44"/>
-      <c r="G9" s="44"/>
-      <c r="H9" s="44"/>
-      <c r="I9" s="44"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
       <c r="J9" s="4"/>
     </row>
     <row r="10" spans="1:15" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="43" t="s">
+      <c r="B10" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="44"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="44"/>
-      <c r="F10" s="44"/>
-      <c r="G10" s="44"/>
-      <c r="H10" s="44"/>
-      <c r="I10" s="44"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
       <c r="J10" s="4"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="39" t="s">
+      <c r="B11" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="39"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
-      <c r="G11" s="39"/>
-      <c r="H11" s="39"/>
-      <c r="I11" s="39"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
       <c r="J11" s="4"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
@@ -9792,12 +9784,12 @@
       <c r="C12" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="40"/>
-      <c r="E12" s="40"/>
-      <c r="F12" s="40"/>
-      <c r="G12" s="40"/>
-      <c r="H12" s="40"/>
-      <c r="I12" s="40"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="34"/>
       <c r="J12" s="4"/>
     </row>
     <row r="13" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9810,12 +9802,12 @@
       <c r="C13" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="41"/>
-      <c r="E13" s="41"/>
-      <c r="F13" s="41"/>
-      <c r="G13" s="41"/>
-      <c r="H13" s="41"/>
-      <c r="I13" s="41"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="35"/>
+      <c r="H13" s="35"/>
+      <c r="I13" s="35"/>
       <c r="J13" s="4"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -9828,12 +9820,12 @@
       <c r="C14" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="41"/>
-      <c r="E14" s="41"/>
-      <c r="F14" s="41"/>
-      <c r="G14" s="41"/>
-      <c r="H14" s="41"/>
-      <c r="I14" s="41"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="35"/>
+      <c r="I14" s="35"/>
       <c r="J14" s="4"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -9846,60 +9838,60 @@
       <c r="C15" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="42"/>
-      <c r="E15" s="42"/>
-      <c r="F15" s="42"/>
-      <c r="G15" s="42"/>
-      <c r="H15" s="42"/>
-      <c r="I15" s="42"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="36"/>
+      <c r="I15" s="36"/>
       <c r="J15" s="4"/>
     </row>
     <row r="16" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="39" t="s">
+      <c r="B16" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="39"/>
-      <c r="F16" s="39"/>
-      <c r="G16" s="39"/>
-      <c r="H16" s="39"/>
-      <c r="I16" s="39"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="33"/>
       <c r="J16" s="4"/>
     </row>
     <row r="17" spans="1:10" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="45" t="s">
+      <c r="B17" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="46"/>
-      <c r="D17" s="46"/>
-      <c r="E17" s="46"/>
-      <c r="F17" s="46"/>
-      <c r="G17" s="46"/>
-      <c r="H17" s="46"/>
-      <c r="I17" s="46"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
       <c r="J17" s="4"/>
     </row>
     <row r="18" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="39" t="s">
+      <c r="B18" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="39"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="39"/>
-      <c r="F18" s="39"/>
-      <c r="G18" s="39"/>
-      <c r="H18" s="39"/>
-      <c r="I18" s="39"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
       <c r="J18" s="4"/>
     </row>
     <row r="19" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -10230,7 +10222,7 @@
         <v>18</v>
       </c>
       <c r="I31" s="19" t="s">
-        <v>2125</v>
+        <v>2122</v>
       </c>
     </row>
     <row r="32" spans="1:10" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.15">
@@ -11336,7 +11328,7 @@
         <v>18</v>
       </c>
       <c r="I75" s="16" t="s">
-        <v>2126</v>
+        <v>2123</v>
       </c>
     </row>
     <row r="76" spans="1:9" ht="150" x14ac:dyDescent="0.25">
@@ -11363,7 +11355,7 @@
         <v>18</v>
       </c>
       <c r="I76" s="16" t="s">
-        <v>2126</v>
+        <v>2123</v>
       </c>
     </row>
     <row r="77" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -18138,7 +18130,7 @@
         <v>941</v>
       </c>
       <c r="C347" s="16" t="s">
-        <v>2124</v>
+        <v>2121</v>
       </c>
       <c r="D347" s="24"/>
       <c r="E347" s="24" t="s">
@@ -22192,7 +22184,7 @@
         <v>1076</v>
       </c>
       <c r="C509" s="16" t="s">
-        <v>2122</v>
+        <v>2119</v>
       </c>
       <c r="D509" s="24"/>
       <c r="E509" s="24" t="s">
@@ -22823,7 +22815,7 @@
         <v>1098</v>
       </c>
       <c r="C534" s="16" t="s">
-        <v>2127</v>
+        <v>2124</v>
       </c>
       <c r="D534" s="17" t="s">
         <v>1704</v>
@@ -22844,13 +22836,13 @@
     </row>
     <row r="535" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A535" s="17" t="s">
-        <v>2129</v>
+        <v>2126</v>
       </c>
       <c r="B535" s="19" t="s">
         <v>1098</v>
       </c>
       <c r="C535" s="16" t="s">
-        <v>2130</v>
+        <v>2127</v>
       </c>
       <c r="D535" s="17" t="s">
         <v>1704</v>
@@ -22928,7 +22920,7 @@
         <v>1098</v>
       </c>
       <c r="C538" s="16" t="s">
-        <v>2128</v>
+        <v>2125</v>
       </c>
       <c r="D538" s="17"/>
       <c r="E538" s="24" t="s">
@@ -22947,13 +22939,13 @@
     </row>
     <row r="539" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A539" s="17" t="s">
-        <v>2131</v>
+        <v>2128</v>
       </c>
       <c r="B539" s="19" t="s">
         <v>1098</v>
       </c>
       <c r="C539" s="16" t="s">
-        <v>2132</v>
+        <v>2129</v>
       </c>
       <c r="D539" s="17"/>
       <c r="E539" s="17" t="s">
@@ -23498,7 +23490,7 @@
         <v>2040</v>
       </c>
     </row>
-    <row r="561" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="561" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A561" s="17" t="s">
         <v>2036</v>
       </c>
@@ -23506,7 +23498,7 @@
         <v>1114</v>
       </c>
       <c r="C561" s="16" t="s">
-        <v>2045</v>
+        <v>2130</v>
       </c>
       <c r="D561" s="29" t="s">
         <v>541</v>
@@ -23803,18 +23795,18 @@
         <v>17</v>
       </c>
       <c r="I572" s="16" t="s">
-        <v>2047</v>
+        <v>2045</v>
       </c>
     </row>
     <row r="573" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A573" s="17" t="s">
-        <v>2046</v>
+        <v>2044</v>
       </c>
       <c r="B573" s="19" t="s">
         <v>1120</v>
       </c>
       <c r="C573" s="16" t="s">
-        <v>2044</v>
+        <v>2131</v>
       </c>
       <c r="D573" s="17" t="s">
         <v>1722</v>
@@ -23941,7 +23933,7 @@
         <v>1123</v>
       </c>
       <c r="C578" s="16" t="s">
-        <v>2048</v>
+        <v>2046</v>
       </c>
       <c r="D578" s="24"/>
       <c r="E578" s="24" t="s">
@@ -23991,7 +23983,7 @@
         <v>1123</v>
       </c>
       <c r="C580" s="16" t="s">
-        <v>2049</v>
+        <v>2047</v>
       </c>
       <c r="D580" s="24"/>
       <c r="E580" s="24" t="s">
@@ -24041,7 +24033,7 @@
         <v>1123</v>
       </c>
       <c r="C582" s="16" t="s">
-        <v>2050</v>
+        <v>2048</v>
       </c>
       <c r="D582" s="24"/>
       <c r="E582" s="24" t="s">
@@ -24082,18 +24074,18 @@
         <v>17</v>
       </c>
       <c r="I583" s="16" t="s">
-        <v>2051</v>
-      </c>
-    </row>
-    <row r="584" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+        <v>2049</v>
+      </c>
+    </row>
+    <row r="584" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A584" s="29" t="s">
-        <v>2121</v>
+        <v>2118</v>
       </c>
       <c r="B584" s="19" t="s">
         <v>1123</v>
       </c>
       <c r="C584" s="16" t="s">
-        <v>2052</v>
+        <v>2132</v>
       </c>
       <c r="D584" s="17" t="s">
         <v>561</v>
@@ -24944,8 +24936,8 @@
       <c r="B618" s="19" t="s">
         <v>1168</v>
       </c>
-      <c r="C618" s="33" t="s">
-        <v>2053</v>
+      <c r="C618" s="16" t="s">
+        <v>2050</v>
       </c>
       <c r="D618" s="24"/>
       <c r="E618" s="24" t="s">
@@ -24958,7 +24950,7 @@
         <v>15</v>
       </c>
       <c r="H618" s="17" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I618" s="26"/>
     </row>
@@ -25186,7 +25178,7 @@
         <v>18</v>
       </c>
       <c r="I627" s="16" t="s">
-        <v>2054</v>
+        <v>2051</v>
       </c>
     </row>
     <row r="628" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -25310,7 +25302,7 @@
         <v>15</v>
       </c>
       <c r="H632" s="17" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I632" s="26"/>
     </row>
@@ -25322,7 +25314,7 @@
         <v>1187</v>
       </c>
       <c r="C633" s="16" t="s">
-        <v>2055</v>
+        <v>2052</v>
       </c>
       <c r="D633" s="24"/>
       <c r="E633" s="24" t="s">
@@ -25372,7 +25364,7 @@
         <v>1187</v>
       </c>
       <c r="C635" s="16" t="s">
-        <v>2056</v>
+        <v>2053</v>
       </c>
       <c r="D635" s="24"/>
       <c r="E635" s="24" t="s">
@@ -25472,7 +25464,7 @@
         <v>1187</v>
       </c>
       <c r="C639" s="16" t="s">
-        <v>2057</v>
+        <v>2054</v>
       </c>
       <c r="D639" s="24"/>
       <c r="E639" s="24" t="s">
@@ -25747,7 +25739,7 @@
         <v>1200</v>
       </c>
       <c r="C650" s="16" t="s">
-        <v>2058</v>
+        <v>2055</v>
       </c>
       <c r="D650" s="29"/>
       <c r="E650" s="24" t="s">
@@ -25763,18 +25755,18 @@
         <v>17</v>
       </c>
       <c r="I650" s="16" t="s">
-        <v>2060</v>
+        <v>2057</v>
       </c>
     </row>
     <row r="651" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A651" s="17" t="s">
-        <v>2059</v>
+        <v>2056</v>
       </c>
       <c r="B651" s="19" t="s">
         <v>1200</v>
       </c>
       <c r="C651" s="16" t="s">
-        <v>2061</v>
+        <v>2058</v>
       </c>
       <c r="D651" s="17" t="s">
         <v>620</v>
@@ -26601,7 +26593,7 @@
         <v>1234</v>
       </c>
       <c r="C684" s="16" t="s">
-        <v>2062</v>
+        <v>2059</v>
       </c>
       <c r="D684" s="24"/>
       <c r="E684" s="24" t="s">
@@ -26626,7 +26618,7 @@
         <v>1234</v>
       </c>
       <c r="C685" s="16" t="s">
-        <v>2063</v>
+        <v>2060</v>
       </c>
       <c r="D685" s="24"/>
       <c r="E685" s="24" t="s">
@@ -26651,7 +26643,7 @@
         <v>1234</v>
       </c>
       <c r="C686" s="16" t="s">
-        <v>2064</v>
+        <v>2061</v>
       </c>
       <c r="D686" s="24"/>
       <c r="E686" s="24" t="s">
@@ -26676,7 +26668,7 @@
         <v>1234</v>
       </c>
       <c r="C687" s="16" t="s">
-        <v>2065</v>
+        <v>2062</v>
       </c>
       <c r="D687" s="24"/>
       <c r="E687" s="24" t="s">
@@ -26701,7 +26693,7 @@
         <v>1234</v>
       </c>
       <c r="C688" s="16" t="s">
-        <v>2066</v>
+        <v>2063</v>
       </c>
       <c r="D688" s="24"/>
       <c r="E688" s="24" t="s">
@@ -26726,7 +26718,7 @@
         <v>1234</v>
       </c>
       <c r="C689" s="16" t="s">
-        <v>2067</v>
+        <v>2064</v>
       </c>
       <c r="D689" s="29"/>
       <c r="E689" s="24" t="s">
@@ -26751,7 +26743,7 @@
         <v>1234</v>
       </c>
       <c r="C690" s="16" t="s">
-        <v>2068</v>
+        <v>2065</v>
       </c>
       <c r="D690" s="24"/>
       <c r="E690" s="24" t="s">
@@ -26776,7 +26768,7 @@
         <v>1234</v>
       </c>
       <c r="C691" s="16" t="s">
-        <v>2069</v>
+        <v>2066</v>
       </c>
       <c r="D691" s="24"/>
       <c r="E691" s="24" t="s">
@@ -26801,7 +26793,7 @@
         <v>1234</v>
       </c>
       <c r="C692" s="16" t="s">
-        <v>2070</v>
+        <v>2067</v>
       </c>
       <c r="D692" s="24"/>
       <c r="E692" s="24" t="s">
@@ -26826,7 +26818,7 @@
         <v>1234</v>
       </c>
       <c r="C693" s="16" t="s">
-        <v>2071</v>
+        <v>2068</v>
       </c>
       <c r="D693" s="24"/>
       <c r="E693" s="24" t="s">
@@ -26851,7 +26843,7 @@
         <v>1234</v>
       </c>
       <c r="C694" s="16" t="s">
-        <v>2072</v>
+        <v>2069</v>
       </c>
       <c r="D694" s="29"/>
       <c r="E694" s="24" t="s">
@@ -27076,7 +27068,7 @@
         <v>1260</v>
       </c>
       <c r="C703" s="16" t="s">
-        <v>2073</v>
+        <v>2070</v>
       </c>
       <c r="D703" s="24"/>
       <c r="E703" s="24" t="s">
@@ -27801,7 +27793,7 @@
         <v>1276</v>
       </c>
       <c r="C732" s="16" t="s">
-        <v>2074</v>
+        <v>2071</v>
       </c>
       <c r="D732" s="24"/>
       <c r="E732" s="24" t="s">
@@ -27976,7 +27968,7 @@
         <v>1284</v>
       </c>
       <c r="C739" s="16" t="s">
-        <v>2075</v>
+        <v>2072</v>
       </c>
       <c r="D739" s="24"/>
       <c r="E739" s="24" t="s">
@@ -27995,13 +27987,13 @@
     </row>
     <row r="740" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A740" s="17" t="s">
-        <v>2077</v>
+        <v>2074</v>
       </c>
       <c r="B740" s="19" t="s">
         <v>1284</v>
       </c>
       <c r="C740" s="16" t="s">
-        <v>2076</v>
+        <v>2073</v>
       </c>
       <c r="D740" s="29"/>
       <c r="E740" s="24" t="s">
@@ -28076,7 +28068,7 @@
         <v>1289</v>
       </c>
       <c r="C743" s="16" t="s">
-        <v>2078</v>
+        <v>2075</v>
       </c>
       <c r="D743" s="24"/>
       <c r="E743" s="24" t="s">
@@ -28101,7 +28093,7 @@
         <v>1289</v>
       </c>
       <c r="C744" s="16" t="s">
-        <v>2079</v>
+        <v>2076</v>
       </c>
       <c r="D744" s="24"/>
       <c r="E744" s="24" t="s">
@@ -28126,7 +28118,7 @@
         <v>1289</v>
       </c>
       <c r="C745" s="16" t="s">
-        <v>2080</v>
+        <v>2077</v>
       </c>
       <c r="D745" s="24"/>
       <c r="E745" s="24" t="s">
@@ -28176,7 +28168,7 @@
         <v>1289</v>
       </c>
       <c r="C747" s="16" t="s">
-        <v>2081</v>
+        <v>2078</v>
       </c>
       <c r="D747" s="24"/>
       <c r="E747" s="24" t="s">
@@ -28201,7 +28193,7 @@
         <v>1289</v>
       </c>
       <c r="C748" s="16" t="s">
-        <v>2082</v>
+        <v>2079</v>
       </c>
       <c r="D748" s="24"/>
       <c r="E748" s="24" t="s">
@@ -28226,7 +28218,7 @@
         <v>1289</v>
       </c>
       <c r="C749" s="16" t="s">
-        <v>2083</v>
+        <v>2080</v>
       </c>
       <c r="D749" s="24"/>
       <c r="E749" s="24" t="s">
@@ -28251,7 +28243,7 @@
         <v>1289</v>
       </c>
       <c r="C750" s="16" t="s">
-        <v>2084</v>
+        <v>2081</v>
       </c>
       <c r="D750" s="24"/>
       <c r="E750" s="24" t="s">
@@ -28276,7 +28268,7 @@
         <v>1289</v>
       </c>
       <c r="C751" s="16" t="s">
-        <v>2085</v>
+        <v>2082</v>
       </c>
       <c r="D751" s="24"/>
       <c r="E751" s="24" t="s">
@@ -28326,7 +28318,7 @@
         <v>1289</v>
       </c>
       <c r="C753" s="16" t="s">
-        <v>2086</v>
+        <v>2083</v>
       </c>
       <c r="D753" s="24"/>
       <c r="E753" s="24" t="s">
@@ -28351,7 +28343,7 @@
         <v>1289</v>
       </c>
       <c r="C754" s="16" t="s">
-        <v>2087</v>
+        <v>2084</v>
       </c>
       <c r="D754" s="24"/>
       <c r="E754" s="24" t="s">
@@ -28376,7 +28368,7 @@
         <v>1289</v>
       </c>
       <c r="C755" s="16" t="s">
-        <v>2088</v>
+        <v>2085</v>
       </c>
       <c r="D755" s="24"/>
       <c r="E755" s="24" t="s">
@@ -28401,7 +28393,7 @@
         <v>1289</v>
       </c>
       <c r="C756" s="16" t="s">
-        <v>2089</v>
+        <v>2086</v>
       </c>
       <c r="D756" s="24"/>
       <c r="E756" s="24" t="s">
@@ -28426,7 +28418,7 @@
         <v>1289</v>
       </c>
       <c r="C757" s="16" t="s">
-        <v>2090</v>
+        <v>2087</v>
       </c>
       <c r="D757" s="24"/>
       <c r="E757" s="24" t="s">
@@ -28501,7 +28493,7 @@
         <v>1289</v>
       </c>
       <c r="C760" s="16" t="s">
-        <v>2091</v>
+        <v>2088</v>
       </c>
       <c r="D760" s="24"/>
       <c r="E760" s="24" t="s">
@@ -28626,7 +28618,7 @@
         <v>1300</v>
       </c>
       <c r="C765" s="16" t="s">
-        <v>2092</v>
+        <v>2089</v>
       </c>
       <c r="D765" s="24"/>
       <c r="E765" s="24" t="s">
@@ -28651,7 +28643,7 @@
         <v>1300</v>
       </c>
       <c r="C766" s="16" t="s">
-        <v>2093</v>
+        <v>2090</v>
       </c>
       <c r="D766" s="24"/>
       <c r="E766" s="24" t="s">
@@ -28676,7 +28668,7 @@
         <v>1300</v>
       </c>
       <c r="C767" s="16" t="s">
-        <v>2094</v>
+        <v>2091</v>
       </c>
       <c r="D767" s="24"/>
       <c r="E767" s="24" t="s">
@@ -28701,7 +28693,7 @@
         <v>1300</v>
       </c>
       <c r="C768" s="16" t="s">
-        <v>2095</v>
+        <v>2092</v>
       </c>
       <c r="D768" s="24"/>
       <c r="E768" s="24" t="s">
@@ -28751,7 +28743,7 @@
         <v>1300</v>
       </c>
       <c r="C770" s="16" t="s">
-        <v>2096</v>
+        <v>2093</v>
       </c>
       <c r="D770" s="24"/>
       <c r="E770" s="24" t="s">
@@ -29089,7 +29081,7 @@
         <v>16</v>
       </c>
       <c r="H783" s="17" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I783" s="26"/>
     </row>
@@ -29326,7 +29318,7 @@
         <v>1321</v>
       </c>
       <c r="C793" s="16" t="s">
-        <v>2097</v>
+        <v>2094</v>
       </c>
       <c r="D793" s="24"/>
       <c r="E793" s="24" t="s">
@@ -29926,7 +29918,7 @@
         <v>1346</v>
       </c>
       <c r="C817" s="16" t="s">
-        <v>2098</v>
+        <v>2095</v>
       </c>
       <c r="D817" s="24"/>
       <c r="E817" s="24" t="s">
@@ -29951,7 +29943,7 @@
         <v>1346</v>
       </c>
       <c r="C818" s="16" t="s">
-        <v>2099</v>
+        <v>2096</v>
       </c>
       <c r="D818" s="24"/>
       <c r="E818" s="24" t="s">
@@ -30201,7 +30193,7 @@
         <v>1356</v>
       </c>
       <c r="C828" s="16" t="s">
-        <v>2100</v>
+        <v>2097</v>
       </c>
       <c r="D828" s="24"/>
       <c r="E828" s="24" t="s">
@@ -30226,7 +30218,7 @@
         <v>1356</v>
       </c>
       <c r="C829" s="16" t="s">
-        <v>2101</v>
+        <v>2098</v>
       </c>
       <c r="D829" s="24"/>
       <c r="E829" s="24" t="s">
@@ -30276,7 +30268,7 @@
         <v>1356</v>
       </c>
       <c r="C831" s="16" t="s">
-        <v>2102</v>
+        <v>2099</v>
       </c>
       <c r="D831" s="24"/>
       <c r="E831" s="24" t="s">
@@ -30301,7 +30293,7 @@
         <v>1356</v>
       </c>
       <c r="C832" s="16" t="s">
-        <v>2103</v>
+        <v>2100</v>
       </c>
       <c r="D832" s="24"/>
       <c r="E832" s="24" t="s">
@@ -30489,7 +30481,7 @@
         <v>15</v>
       </c>
       <c r="H839" s="24" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I839" s="26"/>
     </row>
@@ -31026,7 +31018,7 @@
         <v>1392</v>
       </c>
       <c r="C861" s="16" t="s">
-        <v>2104</v>
+        <v>2101</v>
       </c>
       <c r="D861" s="24"/>
       <c r="E861" s="24" t="s">
@@ -31151,7 +31143,7 @@
         <v>1392</v>
       </c>
       <c r="C866" s="16" t="s">
-        <v>2105</v>
+        <v>2102</v>
       </c>
       <c r="D866" s="24"/>
       <c r="E866" s="24" t="s">
@@ -31201,7 +31193,7 @@
         <v>1392</v>
       </c>
       <c r="C868" s="16" t="s">
-        <v>2106</v>
+        <v>2103</v>
       </c>
       <c r="D868" s="24"/>
       <c r="E868" s="24" t="s">
@@ -31967,7 +31959,7 @@
         <v>18</v>
       </c>
       <c r="I898" s="16" t="s">
-        <v>2120</v>
+        <v>2117</v>
       </c>
     </row>
     <row r="899" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -32003,7 +31995,7 @@
         <v>1432</v>
       </c>
       <c r="C900" s="16" t="s">
-        <v>2107</v>
+        <v>2104</v>
       </c>
       <c r="D900" s="24"/>
       <c r="E900" s="24" t="s">
@@ -32153,7 +32145,7 @@
         <v>1432</v>
       </c>
       <c r="C906" s="16" t="s">
-        <v>2108</v>
+        <v>2105</v>
       </c>
       <c r="D906" s="24"/>
       <c r="E906" s="24" t="s">
@@ -32253,7 +32245,7 @@
         <v>1432</v>
       </c>
       <c r="C910" s="16" t="s">
-        <v>2109</v>
+        <v>2106</v>
       </c>
       <c r="D910" s="24"/>
       <c r="E910" s="24" t="s">
@@ -32344,7 +32336,7 @@
         <v>18</v>
       </c>
       <c r="I913" s="16" t="s">
-        <v>2119</v>
+        <v>2116</v>
       </c>
     </row>
     <row r="914" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -32680,7 +32672,7 @@
         <v>1444</v>
       </c>
       <c r="C927" s="16" t="s">
-        <v>2110</v>
+        <v>2107</v>
       </c>
       <c r="D927" s="24"/>
       <c r="E927" s="24" t="s">
@@ -32730,7 +32722,7 @@
         <v>1444</v>
       </c>
       <c r="C929" s="16" t="s">
-        <v>2111</v>
+        <v>2108</v>
       </c>
       <c r="D929" s="24"/>
       <c r="E929" s="24" t="s">
@@ -32743,7 +32735,7 @@
         <v>15</v>
       </c>
       <c r="H929" s="17" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I929" s="26"/>
     </row>
@@ -32821,7 +32813,7 @@
         <v>18</v>
       </c>
       <c r="I932" s="16" t="s">
-        <v>2117</v>
+        <v>2114</v>
       </c>
     </row>
     <row r="933" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -33573,7 +33565,7 @@
         <v>18</v>
       </c>
       <c r="I962" s="16" t="s">
-        <v>2118</v>
+        <v>2115</v>
       </c>
     </row>
     <row r="963" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -33659,7 +33651,7 @@
         <v>1483</v>
       </c>
       <c r="C966" s="16" t="s">
-        <v>2112</v>
+        <v>2109</v>
       </c>
       <c r="D966" s="24"/>
       <c r="E966" s="24" t="s">
@@ -34250,18 +34242,18 @@
         <v>17</v>
       </c>
       <c r="I989" s="16" t="s">
-        <v>2114</v>
+        <v>2111</v>
       </c>
     </row>
     <row r="990" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A990" s="17" t="s">
-        <v>2113</v>
+        <v>2110</v>
       </c>
       <c r="B990" s="19" t="s">
         <v>1523</v>
       </c>
       <c r="C990" s="16" t="s">
-        <v>2115</v>
+        <v>2112</v>
       </c>
       <c r="D990" s="17" t="s">
         <v>288</v>
@@ -34488,7 +34480,7 @@
         <v>1523</v>
       </c>
       <c r="C999" s="16" t="s">
-        <v>2116</v>
+        <v>2113</v>
       </c>
       <c r="D999" s="24"/>
       <c r="E999" s="24" t="s">
@@ -34682,6 +34674,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -34689,11 +34686,6 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="J257:J260 J262:J265 A20:I28 B29:I46 B244:D244 B242:B243 D242:D243 B248:D248 B245:B247 D245:D247 B252:D252 B249:B251 D249:D251 B253:B255 D253:D255 B256:D272 B275:D276 B273:B274 D273:D274 B277:B278 D277:D278 B377:B382 D377:D382 B440:D457 B430:B439 D430:D439 B460:D485 D458:D459 B488:D491 B486:B487 D486:D487 B492:B494 D492:D494 B383:D429 B458:B459 B547:D558 B543:B546 D543:D546 B565:D568 D559:D564 B559:B564 D569:D573 B569:B573 B574:D577 B578:B580 D578:D580 B581:D617 B618 D618 A619:I632 A636:I638 A633:B635 D633:I635 A640:I644 A639:B639 D639:I639 A647:I649 A645:B646 D645:I646 A650:B650 E650:I650 A684:B694 D684:I694 A703:B703 D703:I703 A704:I731 A732:B733 D732:I733 A734:I742 A746:I746 A743:B745 D743:I745 A752:I752 A747:B751 D747:I751 A758:I759 A753:B757 D753:I757 A761:I763 A760:B760 D760:I760 A769:I769 A764:B768 D764:I768 A772:I792 A770:B771 D770:I771 A793:B793 D793:I793 A794:I813 A815:I816 A814:B814 D814:I814 A819:I827 A817:B818 D817:I818 A833:I860 A828:B832 D828:I832 A862:I865 A861:B861 D861:I861 A867:I867 A866:B866 D866:I866 A869:I899 A868:B868 D868:I868 A901:I905 A900:B900 D900:I900 A908:I909 A906:B907 D906:I907 A914:I926 A910:B913 D910:I913 A928:I928 A927:B927 D927:I927 A930:I931 A929:B929 D929:I929 A933:I965 A932:B932 D932:I932 A966:B966 D966:I966 A991:I998 A990:H990 A967:I989 A1000:I1006 A999:B999 D999:I999 B495:D534 B47:D241 A651:I683 A695:I702 B279:D376 A29:A534 E47:I534 E536:I538 A536:C538 D536 B540:D542 A540:A618 E540:I618">

</xml_diff>

<commit_message>
Update RS and code for MS-ONESTORE release 20250218
</commit_message>
<xml_diff>
--- a/FileSyncandWOPI/Docs/MS-ONESTORE/MS-ONESTORE_RequirementSpecification.xlsx
+++ b/FileSyncandWOPI/Docs/MS-ONESTORE/MS-ONESTORE_RequirementSpecification.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28623"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkSpace\TestSuites\Interop-TestSuites-WJP-Commit\FileSyncandWOPI\Docs\MS-ONESTORE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TestSuite\20250218\Interop-TestSuites\FileSyncandWOPI\Docs\MS-ONESTORE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14567F09-12CC-4BD5-ACF2-02878684F739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{142D57A0-81B8-4D37-B72B-C1A7E204D0B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7053,6 +7053,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -7077,21 +7092,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -7100,14 +7100,14 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <bgColor theme="5" tint="0.59996337778862885"/>
+          <bgColor theme="6" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <bgColor theme="6" tint="0.59996337778862885"/>
+          <bgColor theme="5" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -8811,7 +8811,7 @@
   <dimension ref="A1:O1006"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D981" sqref="D981"/>
+      <selection activeCell="A4" sqref="A4:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -8854,42 +8854,42 @@
         <v>3</v>
       </c>
       <c r="C3" s="9">
-        <v>13.1</v>
+        <v>13.2</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>4</v>
       </c>
       <c r="F3" s="10">
-        <v>45608</v>
+        <v>45706</v>
       </c>
       <c r="J3" s="24"/>
     </row>
     <row r="4" spans="1:15" ht="21">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
       <c r="J4" s="24"/>
     </row>
     <row r="5" spans="1:15">
       <c r="A5" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
       <c r="J5" s="24"/>
       <c r="O5" s="25"/>
     </row>
@@ -8897,96 +8897,96 @@
       <c r="A6" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="38"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
       <c r="J6" s="24"/>
     </row>
     <row r="7" spans="1:15">
       <c r="A7" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="39" t="s">
+      <c r="B7" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="39"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
-      <c r="G7" s="39"/>
-      <c r="H7" s="39"/>
-      <c r="I7" s="39"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="31"/>
       <c r="J7" s="24"/>
     </row>
     <row r="8" spans="1:15">
       <c r="A8" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="39" t="s">
+      <c r="B8" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="39"/>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="39"/>
-      <c r="H8" s="39"/>
-      <c r="I8" s="39"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="31"/>
       <c r="J8" s="24"/>
     </row>
     <row r="9" spans="1:15" ht="78.75" customHeight="1">
       <c r="A9" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="32"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="32"/>
-      <c r="I9" s="32"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="37"/>
+      <c r="I9" s="37"/>
       <c r="J9" s="24"/>
     </row>
     <row r="10" spans="1:15" ht="33.75" customHeight="1">
       <c r="A10" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="31" t="s">
+      <c r="B10" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="32"/>
-      <c r="I10" s="32"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="37"/>
+      <c r="I10" s="37"/>
       <c r="J10" s="24"/>
     </row>
     <row r="11" spans="1:15">
       <c r="A11" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="27"/>
-      <c r="I11" s="27"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="32"/>
       <c r="J11" s="24"/>
     </row>
     <row r="12" spans="1:15">
@@ -8999,12 +8999,12 @@
       <c r="C12" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="28"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="28"/>
-      <c r="I12" s="28"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="33"/>
+      <c r="I12" s="33"/>
       <c r="J12" s="24"/>
     </row>
     <row r="13" spans="1:15" ht="15" customHeight="1">
@@ -9017,12 +9017,12 @@
       <c r="C13" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="29"/>
-      <c r="I13" s="29"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="34"/>
+      <c r="I13" s="34"/>
       <c r="J13" s="24"/>
     </row>
     <row r="14" spans="1:15">
@@ -9035,12 +9035,12 @@
       <c r="C14" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="29"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="29"/>
-      <c r="H14" s="29"/>
-      <c r="I14" s="29"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="34"/>
       <c r="J14" s="24"/>
     </row>
     <row r="15" spans="1:15">
@@ -9053,60 +9053,60 @@
       <c r="C15" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="30"/>
-      <c r="I15" s="30"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="35"/>
+      <c r="I15" s="35"/>
       <c r="J15" s="24"/>
     </row>
     <row r="16" spans="1:15" ht="30" customHeight="1">
       <c r="A16" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="27" t="s">
+      <c r="B16" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="27"/>
-      <c r="H16" s="27"/>
-      <c r="I16" s="27"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="32"/>
       <c r="J16" s="24"/>
     </row>
     <row r="17" spans="1:10" ht="64.5" customHeight="1">
       <c r="A17" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="33" t="s">
+      <c r="B17" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="34"/>
-      <c r="G17" s="34"/>
-      <c r="H17" s="34"/>
-      <c r="I17" s="34"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="39"/>
+      <c r="G17" s="39"/>
+      <c r="H17" s="39"/>
+      <c r="I17" s="39"/>
       <c r="J17" s="24"/>
     </row>
     <row r="18" spans="1:10" ht="30" customHeight="1">
       <c r="A18" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="27" t="s">
+      <c r="B18" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="27"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="27"/>
-      <c r="H18" s="27"/>
-      <c r="I18" s="27"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="32"/>
       <c r="J18" s="24"/>
     </row>
     <row r="19" spans="1:10" ht="30">
@@ -33895,11 +33895,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B5:I5"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B8:I8"/>
     <mergeCell ref="B18:I18"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B9:I9"/>
@@ -33907,34 +33902,39 @@
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="B16:I16"/>
     <mergeCell ref="B17:I17"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B5:I5"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B8:I8"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <conditionalFormatting sqref="A535:B535 D535:I535">
     <cfRule type="expression" dxfId="197" priority="20">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="196" priority="15">
+    <cfRule type="expression" dxfId="196" priority="17">
+      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="195" priority="15">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="195" priority="16">
+    <cfRule type="expression" dxfId="194" priority="16">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="194" priority="17">
-      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A20:I28 B29:I46 A29:A534 B47:D241 E47:I534 B242:B243 D242:D243 B244:D244 B245:B247 D245:D247 B248:D248 B249:B251 D249:D251 B252:D252 B253:B255 D253:D255 B256:D272 J257:J260 J262:J265 B273:B274 D273:D274 B275:D276 B277:B278 D277:D278 B279:D376 B377:B382 D377:D382 B383:D429 B430:B439 D430:D439 B440:D457 B458:B459 D458:D459 B460:D485 B486:B487 D486:D487 B488:D491 B492:B494 D492:D494 B495:D534 A536:C538 E536:I538 B540:D542 A540:A618 E540:I618 B543:B546 D543:D546 B547:D558 B559:B564 D559:D564 B565:D568 B569:B573 D569:D573 B574:D577 B578:B580 D578:D580 B581:D617 B618 D618 A619:I632 A633:B635 D633:I635 A636:I638 A639:B639 D639:I639 A640:I644 A645:B646 D645:I646 A647:I649 A650:B650 E650:I650 A651:I683 A684:B694 D684:I694 A695:I702 A703:B703 D703:I703 A704:I731 A732:B733 D732:I733 A734:I742 A743:B745 D743:I745 A746:I746 A747:B751 D747:I751 A752:I752 A753:B757 D753:I757 A758:I759 A760:B760 D760:I760 A761:I763 A764:B768 D764:I768 A769:I769 A770:B771 D770:I771 A772:I792 A793:B793 D793:I793 A794:I813 A814:B814 D814:I814 A815:I816 A817:B818 D817:I818 A819:I827 A828:B832 D828:I832 A833:I860 A861:B861 D861:I861 A862:I865 A866:B866 D866:I866 A867:I867 A868:B868 D868:I868 A869:I899 A900:B900 D900:I900 A901:I905 A906:B907 D906:I907 A908:I909 A910:B913 D910:I913 A914:I926 A927:B927 D927:I927 A928:I928 A929:B929 D929:I929 A930:I931 A932:B932 D932:I932 A933:I965 A966:B966 D966:I966 A967:I989 A990:H990 A991:I998 A999:B999 D999:I999 A1000:I1006">
-    <cfRule type="expression" dxfId="193" priority="429">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    <cfRule type="expression" dxfId="193" priority="383">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="192" priority="385">
+    <cfRule type="expression" dxfId="192" priority="384">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="191" priority="385">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="191" priority="384">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="190" priority="383">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
+    <cfRule type="expression" dxfId="190" priority="429">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A539:I539">
@@ -33952,17 +33952,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C242:C243">
-    <cfRule type="expression" dxfId="185" priority="320">
+    <cfRule type="expression" dxfId="185" priority="318">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="184" priority="317">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="183" priority="320">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="184" priority="319">
+    <cfRule type="expression" dxfId="182" priority="319">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="183" priority="318">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="182" priority="317">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C245:C247">
@@ -33994,53 +33994,53 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C253:C255">
-    <cfRule type="expression" dxfId="173" priority="302">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="172" priority="301">
+    <cfRule type="expression" dxfId="173" priority="301">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="171" priority="300">
+    <cfRule type="expression" dxfId="172" priority="300">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="170" priority="299">
+    <cfRule type="expression" dxfId="171" priority="299">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="170" priority="302">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C273:C274">
-    <cfRule type="expression" dxfId="169" priority="293">
+    <cfRule type="expression" dxfId="169" priority="294">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="168" priority="293">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="168" priority="296">
+    <cfRule type="expression" dxfId="167" priority="296">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="167" priority="295">
+    <cfRule type="expression" dxfId="166" priority="295">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="166" priority="294">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C277:C278">
-    <cfRule type="expression" dxfId="165" priority="289">
+    <cfRule type="expression" dxfId="165" priority="290">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="164" priority="289">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="164" priority="287">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="163" priority="288">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="162" priority="290">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    <cfRule type="expression" dxfId="162" priority="287">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C377:C382">
-    <cfRule type="expression" dxfId="161" priority="283">
+    <cfRule type="expression" dxfId="161" priority="284">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="160" priority="283">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="160" priority="284">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="159" priority="282">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
@@ -34050,31 +34050,31 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C430:C439">
-    <cfRule type="expression" dxfId="157" priority="275">
+    <cfRule type="expression" dxfId="157" priority="278">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="156" priority="276">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="155" priority="275">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="156" priority="278">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="155" priority="277">
+    <cfRule type="expression" dxfId="154" priority="277">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="154" priority="276">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C458:C459">
-    <cfRule type="expression" dxfId="153" priority="271">
+    <cfRule type="expression" dxfId="153" priority="272">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="152" priority="271">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="152" priority="272">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    <cfRule type="expression" dxfId="151" priority="270">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="151" priority="269">
+    <cfRule type="expression" dxfId="150" priority="269">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="150" priority="270">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C486:C487">
@@ -34092,45 +34092,45 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C492:C494">
-    <cfRule type="expression" dxfId="145" priority="260">
+    <cfRule type="expression" dxfId="145" priority="258">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="144" priority="257">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="143" priority="260">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="144" priority="259">
+    <cfRule type="expression" dxfId="142" priority="259">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="143" priority="258">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C535">
+    <cfRule type="expression" dxfId="141" priority="12">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="140" priority="11">
+      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="139" priority="10">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="142" priority="257">
+    <cfRule type="expression" dxfId="138" priority="9">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C535">
-    <cfRule type="expression" dxfId="141" priority="11">
-      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="140" priority="10">
+  <conditionalFormatting sqref="C543:C546">
+    <cfRule type="expression" dxfId="137" priority="252">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="139" priority="9">
+    <cfRule type="expression" dxfId="136" priority="251">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="138" priority="12">
+    <cfRule type="expression" dxfId="135" priority="254">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C543:C546">
-    <cfRule type="expression" dxfId="137" priority="254">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="136" priority="253">
+    <cfRule type="expression" dxfId="134" priority="253">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="135" priority="252">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="134" priority="251">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C559:C564">
@@ -34148,17 +34148,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C569:C573">
-    <cfRule type="expression" dxfId="129" priority="239">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
+    <cfRule type="expression" dxfId="129" priority="242">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="128" priority="240">
+    <cfRule type="expression" dxfId="128" priority="241">
+      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="127" priority="240">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="127" priority="241">
-      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="126" priority="242">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    <cfRule type="expression" dxfId="126" priority="239">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C578:C580">
@@ -34176,45 +34176,45 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C618">
-    <cfRule type="expression" dxfId="121" priority="229">
+    <cfRule type="expression" dxfId="121" priority="230">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="120" priority="229">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="120" priority="227">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="119" priority="228">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="118" priority="230">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    <cfRule type="expression" dxfId="118" priority="227">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C633:C635">
-    <cfRule type="expression" dxfId="117" priority="223">
-      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="116" priority="224">
+    <cfRule type="expression" dxfId="117" priority="224">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="115" priority="222">
+    <cfRule type="expression" dxfId="116" priority="222">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="115" priority="223">
+      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="114" priority="221">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C639">
-    <cfRule type="expression" dxfId="113" priority="218">
+    <cfRule type="expression" dxfId="113" priority="216">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="112" priority="215">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="111" priority="218">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="112" priority="216">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="111" priority="217">
+    <cfRule type="expression" dxfId="110" priority="217">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="110" priority="215">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C645:C646">
@@ -34232,45 +34232,45 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C650">
-    <cfRule type="expression" dxfId="105" priority="206">
+    <cfRule type="expression" dxfId="105" priority="204">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="104" priority="203">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="103" priority="206">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="104" priority="205">
+    <cfRule type="expression" dxfId="102" priority="205">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="103" priority="204">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="102" priority="203">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C684:C694">
-    <cfRule type="expression" dxfId="101" priority="188">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="100" priority="187">
+    <cfRule type="expression" dxfId="101" priority="187">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="99" priority="186">
+    <cfRule type="expression" dxfId="100" priority="186">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="98" priority="185">
+    <cfRule type="expression" dxfId="99" priority="185">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="98" priority="188">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C703">
-    <cfRule type="expression" dxfId="97" priority="180">
+    <cfRule type="expression" dxfId="97" priority="182">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="96" priority="181">
+      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="95" priority="180">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="96" priority="179">
+    <cfRule type="expression" dxfId="94" priority="179">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="95" priority="181">
-      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="94" priority="182">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C732:C733">
@@ -34291,28 +34291,28 @@
     <cfRule type="expression" dxfId="89" priority="164">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="88" priority="161">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
+    <cfRule type="expression" dxfId="88" priority="163">
+      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="87" priority="162">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="86" priority="163">
-      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
+    <cfRule type="expression" dxfId="86" priority="161">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C747:C751">
-    <cfRule type="expression" dxfId="85" priority="157">
-      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="84" priority="156">
+    <cfRule type="expression" dxfId="85" priority="156">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="83" priority="155">
+    <cfRule type="expression" dxfId="84" priority="155">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="82" priority="158">
+    <cfRule type="expression" dxfId="83" priority="158">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="82" priority="157">
+      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C753:C757">
@@ -34330,199 +34330,199 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C760">
-    <cfRule type="expression" dxfId="77" priority="145">
+    <cfRule type="expression" dxfId="77" priority="146">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="76" priority="145">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="76" priority="144">
+    <cfRule type="expression" dxfId="75" priority="144">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="75" priority="143">
+    <cfRule type="expression" dxfId="74" priority="143">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="74" priority="146">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C764:C768">
-    <cfRule type="expression" dxfId="73" priority="125">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
+    <cfRule type="expression" dxfId="73" priority="128">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="72" priority="126">
+    <cfRule type="expression" dxfId="72" priority="127">
+      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="71" priority="126">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="71" priority="128">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="70" priority="127">
-      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
+    <cfRule type="expression" dxfId="70" priority="125">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C770:C771">
-    <cfRule type="expression" dxfId="69" priority="113">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
+    <cfRule type="expression" dxfId="69" priority="116">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="68" priority="115">
+    <cfRule type="expression" dxfId="68" priority="114">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="67" priority="115">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="67" priority="116">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="66" priority="114">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
+    <cfRule type="expression" dxfId="66" priority="113">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C793">
-    <cfRule type="expression" dxfId="65" priority="108">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
+    <cfRule type="expression" dxfId="65" priority="110">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="64" priority="109">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="63" priority="107">
+    <cfRule type="expression" dxfId="63" priority="108">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="62" priority="107">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="62" priority="110">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C814">
     <cfRule type="expression" dxfId="61" priority="102">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="104">
+    <cfRule type="expression" dxfId="60" priority="101">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="59" priority="104">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="59" priority="101">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="58" priority="103">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C817:C818">
-    <cfRule type="expression" dxfId="57" priority="97">
+    <cfRule type="expression" dxfId="57" priority="98">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="56" priority="97">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="56" priority="96">
+    <cfRule type="expression" dxfId="55" priority="96">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="55" priority="95">
+    <cfRule type="expression" dxfId="54" priority="95">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="54" priority="98">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C828:C832">
-    <cfRule type="expression" dxfId="53" priority="92">
+    <cfRule type="expression" dxfId="53" priority="90">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="52" priority="89">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="51" priority="92">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="91">
+    <cfRule type="expression" dxfId="50" priority="91">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="90">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C861">
+    <cfRule type="expression" dxfId="49" priority="86">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="48" priority="84">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="89">
+    <cfRule type="expression" dxfId="47" priority="83">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="46" priority="85">
+      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C866">
+    <cfRule type="expression" dxfId="45" priority="80">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="44" priority="79">
+      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="43" priority="78">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="42" priority="77">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C861">
-    <cfRule type="expression" dxfId="49" priority="85">
-      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="48" priority="83">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="47" priority="84">
+  <conditionalFormatting sqref="C868">
+    <cfRule type="expression" dxfId="41" priority="72">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="86">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C866">
-    <cfRule type="expression" dxfId="45" priority="77">
+    <cfRule type="expression" dxfId="40" priority="71">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="44" priority="78">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="43" priority="80">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="42" priority="79">
-      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C868">
-    <cfRule type="expression" dxfId="41" priority="71">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="40" priority="74">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="39" priority="73">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="72">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
+    <cfRule type="expression" dxfId="38" priority="74">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C900">
     <cfRule type="expression" dxfId="37" priority="68">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="66">
+    <cfRule type="expression" dxfId="36" priority="67">
+      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="35" priority="66">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="35" priority="67">
-      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="34" priority="65">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C906:C907">
-    <cfRule type="expression" dxfId="33" priority="62">
+    <cfRule type="expression" dxfId="33" priority="60">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="32" priority="59">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="31" priority="62">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="61">
+    <cfRule type="expression" dxfId="30" priority="61">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="60">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C910:C913">
+    <cfRule type="expression" dxfId="29" priority="56">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="28" priority="55">
+      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="27" priority="54">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="59">
+    <cfRule type="expression" dxfId="26" priority="53">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C910:C913">
-    <cfRule type="expression" dxfId="29" priority="54">
+  <conditionalFormatting sqref="C927">
+    <cfRule type="expression" dxfId="25" priority="50">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="24" priority="49">
+      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="23" priority="48">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="53">
+    <cfRule type="expression" dxfId="22" priority="47">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="27" priority="56">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="26" priority="55">
-      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C927">
-    <cfRule type="expression" dxfId="25" priority="48">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="24" priority="47">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="23" priority="50">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="22" priority="49">
-      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C929">
@@ -34540,45 +34540,45 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C932">
-    <cfRule type="expression" dxfId="17" priority="38">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="16" priority="37">
+    <cfRule type="expression" dxfId="17" priority="37">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="36">
+    <cfRule type="expression" dxfId="16" priority="36">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="35">
+    <cfRule type="expression" dxfId="15" priority="35">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="14" priority="38">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C966">
-    <cfRule type="expression" dxfId="13" priority="32">
+    <cfRule type="expression" dxfId="13" priority="30">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="29">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="11" priority="32">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="31">
+    <cfRule type="expression" dxfId="10" priority="31">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="11" priority="30">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="10" priority="29">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C999">
-    <cfRule type="expression" dxfId="9" priority="26">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="8" priority="25">
+    <cfRule type="expression" dxfId="9" priority="25">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="24">
+    <cfRule type="expression" dxfId="8" priority="24">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="23">
+    <cfRule type="expression" dxfId="7" priority="23">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="26">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D536:D538">
@@ -34596,11 +34596,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20:F1006">
-    <cfRule type="expression" dxfId="1" priority="5">
+    <cfRule type="expression" dxfId="1" priority="4">
+      <formula>NOT(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="5">
       <formula>(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="4">
-      <formula>NOT(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="6">

</xml_diff>